<commit_message>
Run ParameterTuning and collect results
</commit_message>
<xml_diff>
--- a/Feature_Extraction_Tuning.xlsx
+++ b/Feature_Extraction_Tuning.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Backup\SelfDrivingNanoDegree\12_ObjectDetection\MySolution\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41591889-20D4-4562-8BE8-FC27D983FD1B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65F2052F-FE7C-44E3-8658-A1923F84E4AD}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{B367B4D4-F857-44C4-B41D-3B2839A5D615}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1041" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1044" uniqueCount="62">
   <si>
     <t>Index</t>
   </si>
@@ -208,6 +208,9 @@
   </si>
   <si>
     <t>Hist + SB + HOG</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -8633,10 +8636,10 @@
   <dimension ref="A1:X91"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B57" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H92" sqref="H92"/>
+      <selection pane="bottomRight" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8780,8 +8783,8 @@
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
-        <f>IF(C3="","",ROW(C3)-2)</f>
-        <v>1</v>
+        <f>IF(C3="","",ROW(C3)-3)</f>
+        <v>0</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>20</v>
@@ -8840,8 +8843,8 @@
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
-        <f t="shared" ref="A4:A67" si="0">IF(C4="","",ROW(C4)-2)</f>
-        <v>2</v>
+        <f t="shared" ref="A4:A67" si="0">IF(C4="","",ROW(C4)-3)</f>
+        <v>1</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>19</v>
@@ -8901,7 +8904,7 @@
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>20</v>
@@ -8961,7 +8964,7 @@
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>20</v>
@@ -9021,7 +9024,7 @@
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>20</v>
@@ -9081,7 +9084,7 @@
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>20</v>
@@ -9141,7 +9144,7 @@
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>20</v>
@@ -9201,7 +9204,7 @@
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>20</v>
@@ -9261,7 +9264,7 @@
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>20</v>
@@ -9321,7 +9324,7 @@
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>20</v>
@@ -9381,7 +9384,7 @@
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>20</v>
@@ -9441,7 +9444,7 @@
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>20</v>
@@ -9501,7 +9504,7 @@
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>20</v>
@@ -9561,7 +9564,7 @@
     <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>20</v>
@@ -9621,7 +9624,7 @@
     <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>20</v>
@@ -9681,7 +9684,7 @@
     <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>20</v>
@@ -9741,7 +9744,7 @@
     <row r="19" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>20</v>
@@ -9801,7 +9804,7 @@
     <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>20</v>
@@ -9861,7 +9864,7 @@
     <row r="21" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>20</v>
@@ -9921,7 +9924,7 @@
     <row r="22" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>20</v>
@@ -9981,7 +9984,7 @@
     <row r="23" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <f t="shared" si="0"/>
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>20</v>
@@ -10041,7 +10044,7 @@
     <row r="24" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>20</v>
@@ -10101,7 +10104,7 @@
     <row r="25" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <f t="shared" si="0"/>
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>20</v>
@@ -10161,7 +10164,7 @@
     <row r="26" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <f t="shared" si="0"/>
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>20</v>
@@ -10221,7 +10224,7 @@
     <row r="27" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
         <f t="shared" si="0"/>
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>20</v>
@@ -10281,7 +10284,7 @@
     <row r="28" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
         <f t="shared" si="0"/>
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>20</v>
@@ -10341,7 +10344,7 @@
     <row r="29" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
         <f t="shared" si="0"/>
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>20</v>
@@ -10401,7 +10404,7 @@
     <row r="30" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
         <f t="shared" si="0"/>
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>20</v>
@@ -10461,7 +10464,7 @@
     <row r="31" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
         <f t="shared" si="0"/>
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B31" s="5" t="s">
         <v>20</v>
@@ -10521,7 +10524,7 @@
     <row r="32" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>20</v>
@@ -10581,7 +10584,7 @@
     <row r="33" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
         <f t="shared" si="0"/>
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B33" s="5" t="s">
         <v>20</v>
@@ -10640,8 +10643,8 @@
     </row>
     <row r="34" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
-        <f>IF(C34="","",ROW(C34)-2)</f>
-        <v>32</v>
+        <f t="shared" si="0"/>
+        <v>31</v>
       </c>
       <c r="B34" s="5" t="s">
         <v>20</v>
@@ -10700,8 +10703,8 @@
     </row>
     <row r="35" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
-        <f>IF(C35="","",ROW(C35)-2)</f>
-        <v>33</v>
+        <f t="shared" si="0"/>
+        <v>32</v>
       </c>
       <c r="B35" s="5" t="s">
         <v>20</v>
@@ -10761,7 +10764,7 @@
     <row r="36" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
         <f t="shared" si="0"/>
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B36" s="5" t="s">
         <v>19</v>
@@ -10821,7 +10824,7 @@
     <row r="37" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A37" s="5">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B37" s="5" t="s">
         <v>20</v>
@@ -10881,7 +10884,7 @@
     <row r="38" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
         <f t="shared" si="0"/>
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B38" s="5" t="s">
         <v>20</v>
@@ -10941,7 +10944,7 @@
     <row r="39" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A39" s="5">
         <f t="shared" si="0"/>
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B39" s="5" t="s">
         <v>20</v>
@@ -11001,7 +11004,7 @@
     <row r="40" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A40" s="5">
         <f t="shared" si="0"/>
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B40" s="5" t="s">
         <v>20</v>
@@ -11061,7 +11064,7 @@
     <row r="41" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A41" s="5">
         <f t="shared" si="0"/>
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B41" s="5" t="s">
         <v>20</v>
@@ -11121,7 +11124,7 @@
     <row r="42" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A42" s="5">
         <f t="shared" si="0"/>
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B42" s="5" t="s">
         <v>20</v>
@@ -11181,7 +11184,7 @@
     <row r="43" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A43" s="5">
         <f t="shared" si="0"/>
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B43" s="5" t="s">
         <v>20</v>
@@ -11241,7 +11244,7 @@
     <row r="44" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A44" s="5">
         <f t="shared" si="0"/>
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B44" s="5" t="s">
         <v>20</v>
@@ -11301,7 +11304,7 @@
     <row r="45" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A45" s="5">
         <f t="shared" si="0"/>
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B45" s="5" t="s">
         <v>19</v>
@@ -11354,6 +11357,15 @@
       <c r="R45" s="5"/>
       <c r="S45" s="5"/>
       <c r="T45" s="5"/>
+      <c r="U45" s="1">
+        <v>0</v>
+      </c>
+      <c r="V45" s="1">
+        <v>0</v>
+      </c>
+      <c r="W45" s="1">
+        <v>864</v>
+      </c>
       <c r="X45" s="4" t="s">
         <v>31</v>
       </c>
@@ -11361,7 +11373,7 @@
     <row r="46" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A46" s="5">
         <f t="shared" si="0"/>
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B46" s="5" t="s">
         <v>20</v>
@@ -11414,6 +11426,15 @@
       <c r="R46" s="5"/>
       <c r="S46" s="5"/>
       <c r="T46" s="5"/>
+      <c r="U46" s="1">
+        <v>0</v>
+      </c>
+      <c r="V46" s="1">
+        <v>0</v>
+      </c>
+      <c r="W46" s="1">
+        <v>432</v>
+      </c>
       <c r="X46" s="9" t="s">
         <v>46</v>
       </c>
@@ -11421,7 +11442,7 @@
     <row r="47" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A47" s="5">
         <f t="shared" si="0"/>
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B47" s="5" t="s">
         <v>20</v>
@@ -11474,6 +11495,15 @@
       <c r="R47" s="5"/>
       <c r="S47" s="5"/>
       <c r="T47" s="5"/>
+      <c r="U47" s="1">
+        <v>0</v>
+      </c>
+      <c r="V47" s="1">
+        <v>0</v>
+      </c>
+      <c r="W47" s="1">
+        <v>1728</v>
+      </c>
       <c r="X47" s="9" t="s">
         <v>47</v>
       </c>
@@ -11481,7 +11511,7 @@
     <row r="48" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A48" s="5">
         <f t="shared" si="0"/>
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B48" s="5" t="s">
         <v>20</v>
@@ -11531,9 +11561,24 @@
       <c r="Q48" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="R48" s="5"/>
-      <c r="S48" s="5"/>
-      <c r="T48" s="5"/>
+      <c r="R48" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="S48" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="T48" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="U48" s="1">
+        <v>0</v>
+      </c>
+      <c r="V48" s="1">
+        <v>0</v>
+      </c>
+      <c r="W48" s="1">
+        <v>21600</v>
+      </c>
       <c r="X48" s="9" t="s">
         <v>48</v>
       </c>
@@ -11541,7 +11586,7 @@
     <row r="49" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A49" s="5">
         <f t="shared" si="0"/>
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B49" s="5" t="s">
         <v>20</v>
@@ -11574,7 +11619,7 @@
         <v>8</v>
       </c>
       <c r="L49" s="5">
-        <v>64</v>
+        <v>32</v>
       </c>
       <c r="M49" s="5">
         <v>2</v>
@@ -11594,6 +11639,15 @@
       <c r="R49" s="5"/>
       <c r="S49" s="5"/>
       <c r="T49" s="5"/>
+      <c r="U49" s="1">
+        <v>0</v>
+      </c>
+      <c r="V49" s="1">
+        <v>0</v>
+      </c>
+      <c r="W49" s="1">
+        <v>96</v>
+      </c>
       <c r="X49" s="9" t="s">
         <v>49</v>
       </c>
@@ -11601,7 +11655,7 @@
     <row r="50" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A50" s="5">
         <f t="shared" si="0"/>
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B50" s="5" t="s">
         <v>20</v>
@@ -11654,6 +11708,15 @@
       <c r="R50" s="5"/>
       <c r="S50" s="5"/>
       <c r="T50" s="5"/>
+      <c r="U50" s="1">
+        <v>0</v>
+      </c>
+      <c r="V50" s="1">
+        <v>0</v>
+      </c>
+      <c r="W50" s="1">
+        <v>384</v>
+      </c>
       <c r="X50" s="9" t="s">
         <v>50</v>
       </c>
@@ -11661,7 +11724,7 @@
     <row r="51" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A51" s="5">
         <f t="shared" si="0"/>
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B51" s="5" t="s">
         <v>20</v>
@@ -11714,6 +11777,15 @@
       <c r="R51" s="5"/>
       <c r="S51" s="5"/>
       <c r="T51" s="5"/>
+      <c r="U51" s="1">
+        <v>0</v>
+      </c>
+      <c r="V51" s="1">
+        <v>0</v>
+      </c>
+      <c r="W51" s="1">
+        <v>384</v>
+      </c>
       <c r="X51" s="9" t="s">
         <v>51</v>
       </c>
@@ -11721,7 +11793,7 @@
     <row r="52" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A52" s="5">
         <f t="shared" si="0"/>
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B52" s="5" t="s">
         <v>20</v>
@@ -11781,7 +11853,7 @@
     <row r="53" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A53" s="5">
         <f t="shared" si="0"/>
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B53" s="5" t="s">
         <v>20</v>
@@ -11841,7 +11913,7 @@
     <row r="54" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A54" s="5">
         <f t="shared" si="0"/>
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B54" s="5" t="s">
         <v>20</v>
@@ -11901,7 +11973,7 @@
     <row r="55" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A55" s="5">
         <f t="shared" si="0"/>
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B55" s="5" t="s">
         <v>20</v>
@@ -11961,7 +12033,7 @@
     <row r="56" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A56" s="5">
         <f t="shared" si="0"/>
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B56" s="5" t="s">
         <v>20</v>
@@ -12021,7 +12093,7 @@
     <row r="57" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A57" s="5">
         <f t="shared" si="0"/>
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B57" s="5" t="s">
         <v>20</v>
@@ -12081,7 +12153,7 @@
     <row r="58" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A58" s="5">
         <f t="shared" si="0"/>
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B58" s="5" t="s">
         <v>20</v>
@@ -12141,7 +12213,7 @@
     <row r="59" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A59" s="5">
         <f t="shared" si="0"/>
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B59" s="5" t="s">
         <v>20</v>
@@ -12201,7 +12273,7 @@
     <row r="60" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A60" s="5">
         <f t="shared" si="0"/>
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B60" s="5" t="s">
         <v>20</v>
@@ -12261,7 +12333,7 @@
     <row r="61" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A61" s="5">
         <f t="shared" si="0"/>
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B61" s="5" t="s">
         <v>20</v>
@@ -12318,7 +12390,7 @@
     <row r="62" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A62" s="5">
         <f t="shared" si="0"/>
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B62" s="5" t="s">
         <v>20</v>
@@ -12375,7 +12447,7 @@
     <row r="63" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A63" s="5">
         <f t="shared" si="0"/>
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B63" s="5" t="s">
         <v>20</v>
@@ -12432,7 +12504,7 @@
     <row r="64" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A64" s="5">
         <f t="shared" si="0"/>
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B64" s="5" t="s">
         <v>20</v>
@@ -12489,7 +12561,7 @@
     <row r="65" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A65" s="5">
         <f t="shared" si="0"/>
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B65" s="5" t="s">
         <v>20</v>
@@ -12546,7 +12618,7 @@
     <row r="66" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A66" s="5">
         <f t="shared" si="0"/>
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B66" s="5" t="s">
         <v>20</v>
@@ -12603,7 +12675,7 @@
     <row r="67" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A67" s="5">
         <f t="shared" si="0"/>
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B67" s="5" t="s">
         <v>20</v>
@@ -12659,8 +12731,8 @@
     </row>
     <row r="68" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A68" s="5">
-        <f t="shared" ref="A68:A91" si="1">IF(C68="","",ROW(C68)-2)</f>
-        <v>66</v>
+        <f t="shared" ref="A68:A91" si="1">IF(C68="","",ROW(C68)-3)</f>
+        <v>65</v>
       </c>
       <c r="B68" s="5" t="s">
         <v>20</v>
@@ -12717,7 +12789,7 @@
     <row r="69" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A69" s="5">
         <f t="shared" si="1"/>
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B69" s="5" t="s">
         <v>20</v>
@@ -12774,7 +12846,7 @@
     <row r="70" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A70" s="5">
         <f t="shared" si="1"/>
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B70" s="5" t="s">
         <v>20</v>
@@ -12831,7 +12903,7 @@
     <row r="71" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A71" s="5">
         <f t="shared" si="1"/>
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B71" s="5" t="s">
         <v>20</v>
@@ -12888,7 +12960,7 @@
     <row r="72" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A72" s="5">
         <f t="shared" si="1"/>
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B72" s="5" t="s">
         <v>20</v>
@@ -12945,7 +13017,7 @@
     <row r="73" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A73" s="5">
         <f t="shared" si="1"/>
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B73" s="5" t="s">
         <v>20</v>
@@ -13002,7 +13074,7 @@
     <row r="74" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A74" s="5">
         <f t="shared" si="1"/>
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B74" s="5" t="s">
         <v>20</v>
@@ -13059,7 +13131,7 @@
     <row r="75" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A75" s="5">
         <f t="shared" si="1"/>
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B75" s="5" t="s">
         <v>20</v>
@@ -13116,7 +13188,7 @@
     <row r="76" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A76" s="5">
         <f t="shared" si="1"/>
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B76" s="5" t="s">
         <v>20</v>
@@ -13173,7 +13245,7 @@
     <row r="77" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A77" s="5">
         <f t="shared" si="1"/>
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B77" s="5" t="s">
         <v>20</v>
@@ -13230,7 +13302,7 @@
     <row r="78" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A78" s="5">
         <f t="shared" si="1"/>
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B78" s="5" t="s">
         <v>20</v>
@@ -13287,7 +13359,7 @@
     <row r="79" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A79" s="5">
         <f t="shared" si="1"/>
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B79" s="5" t="s">
         <v>20</v>
@@ -13344,7 +13416,7 @@
     <row r="80" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A80" s="5">
         <f t="shared" si="1"/>
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B80" s="5" t="s">
         <v>20</v>
@@ -13401,7 +13473,7 @@
     <row r="81" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A81" s="5">
         <f t="shared" si="1"/>
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B81" s="5" t="s">
         <v>20</v>
@@ -13458,7 +13530,7 @@
     <row r="82" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A82" s="5">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B82" s="5" t="s">
         <v>20</v>
@@ -13515,7 +13587,7 @@
     <row r="83" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A83" s="5">
         <f t="shared" si="1"/>
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B83" s="5" t="s">
         <v>20</v>
@@ -13572,7 +13644,7 @@
     <row r="84" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A84" s="5">
         <f t="shared" si="1"/>
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B84" s="5" t="s">
         <v>20</v>
@@ -13629,7 +13701,7 @@
     <row r="85" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A85" s="5">
         <f t="shared" si="1"/>
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B85" s="5" t="s">
         <v>19</v>
@@ -13686,7 +13758,7 @@
     <row r="86" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A86" s="5">
         <f t="shared" si="1"/>
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B86" s="5" t="s">
         <v>20</v>
@@ -13743,7 +13815,7 @@
     <row r="87" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A87" s="5">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B87" s="5" t="s">
         <v>19</v>
@@ -13800,7 +13872,7 @@
     <row r="88" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A88" s="5">
         <f t="shared" si="1"/>
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B88" s="5" t="s">
         <v>20</v>
@@ -13857,7 +13929,7 @@
     <row r="89" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A89" s="5">
         <f t="shared" si="1"/>
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B89" s="5" t="s">
         <v>19</v>
@@ -13914,7 +13986,7 @@
     <row r="90" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A90" s="5">
         <f t="shared" si="1"/>
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B90" s="5" t="s">
         <v>20</v>
@@ -13971,7 +14043,7 @@
     <row r="91" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A91" s="5">
         <f t="shared" si="1"/>
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B91" s="5" t="s">
         <v>19</v>

</xml_diff>